<commit_message>
repotes: inspeccion consulta de datos ok
</commit_message>
<xml_diff>
--- a/public/Reporte Inspeccion.xlsx
+++ b/public/Reporte Inspeccion.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
   <si>
     <t>NTS N° 198 - MINSA/DIGESA-2023</t>
   </si>
@@ -29,6 +29,12 @@
     <t>INSPECCIÓN DE VIVIENDAS PARA LA VIGILANCIA Y CONTROL DEL Aedes aegypti</t>
   </si>
   <si>
+    <t>CENTRO ESSALUD 1SECTOR 123</t>
+  </si>
+  <si>
+    <t>FERNANDEZ MAURICIO LORENZO</t>
+  </si>
+  <si>
     <t>N°</t>
   </si>
   <si>
@@ -48,6 +54,18 @@
   </si>
   <si>
     <t>Consumo de Larvicida(g)</t>
+  </si>
+  <si>
+    <t>we</t>
+  </si>
+  <si>
+    <t>dfg</t>
+  </si>
+  <si>
+    <t>juana</t>
+  </si>
+  <si>
+    <t>ana</t>
   </si>
   <si>
     <t>&gt; 500 L</t>
@@ -612,23 +630,31 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:44" customHeight="1" ht="28"/>
-    <row r="8" spans="1:44" customHeight="1" ht="28"/>
+    <row r="7" spans="1:44" customHeight="1" ht="28">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:44" customHeight="1" ht="28">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="9" spans="1:44">
       <c r="A9" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -668,10 +694,10 @@
       <c r="AO9" s="4"/>
       <c r="AP9" s="4"/>
       <c r="AQ9" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AR9" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:44">
@@ -680,7 +706,7 @@
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -690,44 +716,44 @@
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
       <c r="U10" s="4" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
       <c r="Y10" s="4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="Z10" s="4"/>
       <c r="AA10" s="4"/>
       <c r="AB10" s="4"/>
       <c r="AC10" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="AD10" s="4"/>
       <c r="AE10" s="4"/>
       <c r="AF10" s="4"/>
       <c r="AG10" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="AH10" s="4"/>
       <c r="AI10" s="4"/>
       <c r="AJ10" s="4"/>
       <c r="AK10" s="4"/>
       <c r="AL10" s="4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="AM10" s="4"/>
       <c r="AN10" s="4"/>
@@ -742,31 +768,31 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
       <c r="U11" s="4" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="V11" s="4"/>
       <c r="W11" s="4"/>
@@ -798,133 +824,147 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="S12" s="4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="T12" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="U12" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="V12" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="W12" s="4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="X12" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="Y12" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="Z12" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="AA12" s="4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="AB12" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="AC12" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="AD12" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="AE12" s="4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="AF12" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="AG12" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="AH12" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="AI12" s="4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="AJ12" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="AK12" s="4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="AL12" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="AM12" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="AN12" s="4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="AO12" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="AP12" s="4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="AQ12" s="4"/>
       <c r="AR12" s="4"/>
     </row>
     <row r="13" spans="1:44">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="A13" s="4">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="4">
+        <v>14</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
+      <c r="I13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
@@ -961,12 +1001,24 @@
       <c r="AR13" s="4"/>
     </row>
     <row r="14" spans="1:44">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+      <c r="A14" s="4">
+        <v>2</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="4">
+        <v>6</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -2066,7 +2118,7 @@
     </row>
     <row r="38" spans="1:44">
       <c r="A38" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>

</xml_diff>

<commit_message>
reportes: inspeccion vista ok y descargar excel ok
</commit_message>
<xml_diff>
--- a/public/Reporte Inspeccion.xlsx
+++ b/public/Reporte Inspeccion.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
   <si>
     <t>NTS N° 198 - MINSA/DIGESA-2023</t>
   </si>
@@ -29,10 +29,10 @@
     <t>INSPECCIÓN DE VIVIENDAS PARA LA VIGILANCIA Y CONTROL DEL Aedes aegypti</t>
   </si>
   <si>
-    <t>CENTRO ESSALUD 1SECTOR 123</t>
-  </si>
-  <si>
-    <t>FERNANDEZ MAURICIO LORENZO</t>
+    <t>dfgdfNUEVO NNN</t>
+  </si>
+  <si>
+    <t>SDFSDFDS</t>
   </si>
   <si>
     <t>N°</t>
@@ -54,18 +54,6 @@
   </si>
   <si>
     <t>Consumo de Larvicida(g)</t>
-  </si>
-  <si>
-    <t>we</t>
-  </si>
-  <si>
-    <t>dfg</t>
-  </si>
-  <si>
-    <t>juana</t>
-  </si>
-  <si>
-    <t>ana</t>
   </si>
   <si>
     <t>&gt; 500 L</t>
@@ -697,7 +685,7 @@
         <v>12</v>
       </c>
       <c r="AR9" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:44">
@@ -706,7 +694,7 @@
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -716,44 +704,44 @@
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
       <c r="U10" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
       <c r="Y10" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="Z10" s="4"/>
       <c r="AA10" s="4"/>
       <c r="AB10" s="4"/>
       <c r="AC10" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="AD10" s="4"/>
       <c r="AE10" s="4"/>
       <c r="AF10" s="4"/>
       <c r="AG10" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AH10" s="4"/>
       <c r="AI10" s="4"/>
       <c r="AJ10" s="4"/>
       <c r="AK10" s="4"/>
       <c r="AL10" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AM10" s="4"/>
       <c r="AN10" s="4"/>
@@ -768,31 +756,31 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
       <c r="U11" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="V11" s="4"/>
       <c r="W11" s="4"/>
@@ -824,147 +812,133 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="S12" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="T12" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="U12" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="V12" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="W12" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="X12" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="Y12" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="Z12" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="AA12" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="AB12" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="AC12" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="AD12" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="AE12" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="AF12" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="AG12" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="AH12" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="AI12" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="AJ12" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="AK12" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="AL12" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="AM12" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="AN12" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="AO12" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="AP12" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="AQ12" s="4"/>
       <c r="AR12" s="4"/>
     </row>
     <row r="13" spans="1:44">
-      <c r="A13" s="4">
-        <v>1</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="4">
-        <v>14</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
@@ -1001,24 +975,12 @@
       <c r="AR13" s="4"/>
     </row>
     <row r="14" spans="1:44">
-      <c r="A14" s="4">
-        <v>2</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="4">
-        <v>6</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>

</xml_diff>

<commit_message>
inpecion y control: vista de imagenes ok
</commit_message>
<xml_diff>
--- a/public/Reporte Inspeccion.xlsx
+++ b/public/Reporte Inspeccion.xlsx
@@ -1241,7 +1241,9 @@
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
+      <c r="I13" s="9">
+        <v>5</v>
+      </c>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
@@ -1254,9 +1256,7 @@
       <c r="S13" s="9"/>
       <c r="T13" s="9"/>
       <c r="U13" s="9"/>
-      <c r="V13" s="9">
-        <v>5</v>
-      </c>
+      <c r="V13" s="9"/>
       <c r="W13" s="9"/>
       <c r="X13" s="9"/>
       <c r="Y13" s="9"/>
@@ -2411,7 +2411,7 @@
       </c>
       <c r="I38" s="10">
         <f>SUM(I13:I37)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J38" s="10">
         <f>SUM(J13:J37)</f>
@@ -2463,7 +2463,7 @@
       </c>
       <c r="V38" s="10">
         <f>SUM(V13:V37)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="W38" s="10">
         <f>SUM(W13:W37)</f>

</xml_diff>

<commit_message>
reportes: inspeccion y control ok
</commit_message>
<xml_diff>
--- a/public/Reporte Inspeccion.xlsx
+++ b/public/Reporte Inspeccion.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
   <si>
     <t>NTS N° 198 - MINSA/DIGESA-2023</t>
   </si>
@@ -35,13 +35,13 @@
     <t>NOMBRES Y APELLIDOS DEL INSPECTOR:</t>
   </si>
   <si>
-    <t>Localidad 2</t>
-  </si>
-  <si>
-    <t>FERNANDEZ MAURICIO LORENZO</t>
-  </si>
-  <si>
-    <t>CENTRO ESSALUD 1</t>
+    <t>VICE</t>
+  </si>
+  <si>
+    <t>SDFSDFDS</t>
+  </si>
+  <si>
+    <t>dfgdf</t>
   </si>
   <si>
     <t>SECTOR:</t>
@@ -50,7 +50,7 @@
     <t>ACTIVIDAD:</t>
   </si>
   <si>
-    <t>SECTOR 123</t>
+    <t>NUEVO NNN</t>
   </si>
   <si>
     <t>VIGILANCIA</t>
@@ -59,18 +59,21 @@
     <t>CONTROL</t>
   </si>
   <si>
+    <t>RECUPERACIÓN</t>
+  </si>
+  <si>
+    <t>FECHA:</t>
+  </si>
+  <si>
+    <t>CERCO</t>
+  </si>
+  <si>
+    <t>28/05/2024</t>
+  </si>
+  <si>
     <t>X</t>
   </si>
   <si>
-    <t>RECUPERACIÓN</t>
-  </si>
-  <si>
-    <t>FECHA:</t>
-  </si>
-  <si>
-    <t>CERCO</t>
-  </si>
-  <si>
     <t>N°</t>
   </si>
   <si>
@@ -146,13 +149,155 @@
     <t>Febriles</t>
   </si>
   <si>
-    <t>we</t>
-  </si>
-  <si>
-    <t>juana</t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Consolidado</t>
+  </si>
+  <si>
+    <t>Abreriaturas</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"/>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="true"/>
+        <i val="false"/>
+        <strike val="false"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+        <u val="none"/>
+      </rPr>
+      <t xml:space="preserve">Viviendas: </t>
+    </r>
+    <r>
+      <t xml:space="preserve">si la vivienda no se pudo inspeccionar consignar C(vivienda cerrada), R(vivienda renuente) o D(vivienda deshabitada).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"/>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="true"/>
+        <i val="false"/>
+        <strike val="false"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+        <u val="none"/>
+      </rPr>
+      <t xml:space="preserve">Depositos: </t>
+    </r>
+    <r>
+      <t xml:space="preserve">en la columna: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="true"/>
+        <i val="false"/>
+        <strike val="false"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+        <u val="none"/>
+      </rPr>
+      <t xml:space="preserve">I</t>
+    </r>
+    <r>
+      <t xml:space="preserve">(inspeccionado), </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="true"/>
+        <i val="false"/>
+        <strike val="false"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+        <u val="none"/>
+      </rPr>
+      <t xml:space="preserve">P</t>
+    </r>
+    <r>
+      <t xml:space="preserve">(positivo), </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="true"/>
+        <i val="false"/>
+        <strike val="false"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+        <u val="none"/>
+      </rPr>
+      <t xml:space="preserve">TQ</t>
+    </r>
+    <r>
+      <t xml:space="preserve">(tratamiento fisico), </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="true"/>
+        <i val="false"/>
+        <strike val="false"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+        <u val="none"/>
+      </rPr>
+      <t xml:space="preserve">D</t>
+    </r>
+    <r>
+      <t xml:space="preserve">(destruido), </t>
+    </r>
+    <r>
+      <t xml:space="preserve">colocar el número de recipientes segun corresponda.</t>
+    </r>
+  </si>
+  <si>
+    <t>Hora de ingreso</t>
+  </si>
+  <si>
+    <t>Hora de salida</t>
+  </si>
+  <si>
+    <t>FIRMA DEL JEFE DE BRIGADA</t>
+  </si>
+  <si>
+    <t>FIRMA DEL JEFE DEL INSPECTOR</t>
+  </si>
+  <si>
+    <t>viviendas inspeccionadas</t>
+  </si>
+  <si>
+    <t>viviendas cerradas</t>
+  </si>
+  <si>
+    <t>viviendas renuentes</t>
+  </si>
+  <si>
+    <t>viviendas deshabitadas</t>
+  </si>
+  <si>
+    <t>viviendas tratadas</t>
+  </si>
+  <si>
+    <t>viviendas positivas</t>
+  </si>
+  <si>
+    <t>recipientes positivos</t>
   </si>
 </sst>
 </file>
@@ -233,7 +378,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -265,11 +410,161 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="25">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -303,6 +598,23 @@
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="3" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="4" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="5" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="6" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="7" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="8" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="9" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="10" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="11" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="12" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="8" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -638,10 +950,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AR38"/>
+  <dimension ref="A1:AR47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A38" sqref="A38:AR38"/>
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -758,12 +1070,14 @@
       <c r="AG5" s="6"/>
       <c r="AH5" s="4"/>
       <c r="AI5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AJ5" s="4"/>
       <c r="AK5" s="4"/>
       <c r="AL5" s="4"/>
-      <c r="AM5" s="5"/>
+      <c r="AM5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AN5" s="6"/>
       <c r="AO5" s="6"/>
       <c r="AP5" s="6"/>
@@ -856,12 +1170,10 @@
       </c>
       <c r="AB7" s="4"/>
       <c r="AC7" s="4"/>
-      <c r="AD7" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="AD7" s="7"/>
       <c r="AE7" s="4"/>
       <c r="AF7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AG7" s="4"/>
       <c r="AH7" s="4"/>
@@ -869,11 +1181,13 @@
       <c r="AJ7" s="7"/>
       <c r="AK7" s="4"/>
       <c r="AL7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AM7" s="4"/>
       <c r="AN7" s="4"/>
-      <c r="AO7" s="7"/>
+      <c r="AO7" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="AP7" s="4"/>
       <c r="AQ7" s="4"/>
       <c r="AR7" s="4"/>
@@ -926,19 +1240,19 @@
     </row>
     <row r="9" spans="1:44">
       <c r="A9" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
@@ -978,10 +1292,10 @@
       <c r="AO9" s="10"/>
       <c r="AP9" s="10"/>
       <c r="AQ9" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AR9" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:44">
@@ -990,7 +1304,7 @@
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
@@ -1000,44 +1314,44 @@
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
       <c r="M10" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
       <c r="P10" s="10"/>
       <c r="Q10" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
       <c r="U10" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="V10" s="10"/>
       <c r="W10" s="10"/>
       <c r="X10" s="10"/>
       <c r="Y10" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Z10" s="10"/>
       <c r="AA10" s="10"/>
       <c r="AB10" s="10"/>
       <c r="AC10" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AD10" s="10"/>
       <c r="AE10" s="10"/>
       <c r="AF10" s="10"/>
       <c r="AG10" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AH10" s="10"/>
       <c r="AI10" s="10"/>
       <c r="AJ10" s="10"/>
       <c r="AK10" s="10"/>
       <c r="AL10" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AM10" s="10"/>
       <c r="AN10" s="10"/>
@@ -1052,31 +1366,31 @@
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
       <c r="Q11" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
       <c r="U11" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="V11" s="10"/>
       <c r="W11" s="10"/>
@@ -1108,118 +1422,118 @@
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F12" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="J12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="K12" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="I12" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="J12" s="10" t="s">
+      <c r="L12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="M12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="K12" s="10" t="s">
+      <c r="N12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="L12" s="10" t="s">
+      <c r="O12" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="M12" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N12" s="10" t="s">
+      <c r="P12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="O12" s="10" t="s">
+      <c r="R12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="P12" s="10" t="s">
+      <c r="S12" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="Q12" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="R12" s="10" t="s">
+      <c r="T12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="U12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="S12" s="10" t="s">
+      <c r="V12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="T12" s="10" t="s">
+      <c r="W12" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="U12" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="V12" s="10" t="s">
+      <c r="X12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="W12" s="10" t="s">
+      <c r="Z12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="X12" s="10" t="s">
+      <c r="AA12" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="Y12" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z12" s="10" t="s">
+      <c r="AB12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="AA12" s="10" t="s">
+      <c r="AD12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="AB12" s="10" t="s">
+      <c r="AE12" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="AC12" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD12" s="10" t="s">
+      <c r="AF12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="AE12" s="10" t="s">
+      <c r="AH12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="AF12" s="10" t="s">
+      <c r="AI12" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="AG12" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="AH12" s="10" t="s">
+      <c r="AJ12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="AK12" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AL12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="AI12" s="10" t="s">
+      <c r="AM12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="AJ12" s="10" t="s">
+      <c r="AN12" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="AK12" s="10" t="s">
+      <c r="AO12" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="AL12" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM12" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="AN12" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="AO12" s="10" t="s">
-        <v>40</v>
-      </c>
       <c r="AP12" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AQ12" s="10"/>
       <c r="AR12" s="10"/>
@@ -1229,22 +1543,26 @@
         <v>1</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D13" s="9">
+        <v>8</v>
+      </c>
+      <c r="E13" s="9">
         <v>14</v>
       </c>
-      <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9">
-        <v>5</v>
-      </c>
-      <c r="J13" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="J13" s="9">
+        <v>3</v>
+      </c>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
@@ -1278,7 +1596,7 @@
       <c r="AO13" s="9"/>
       <c r="AP13" s="9"/>
       <c r="AQ13" s="9">
-        <v>5.0</v>
+        <v>14.0</v>
       </c>
       <c r="AR13" s="9"/>
     </row>
@@ -2388,14 +2706,14 @@
     </row>
     <row r="38" spans="1:44">
       <c r="A38" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
       <c r="E38" s="10">
         <f>SUM(E13:E37)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F38" s="10">
         <f>SUM(F13:F37)</f>
@@ -2411,11 +2729,11 @@
       </c>
       <c r="I38" s="10">
         <f>SUM(I13:I37)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J38" s="10">
         <f>SUM(J13:J37)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K38" s="10">
         <f>SUM(K13:K37)</f>
@@ -2547,9 +2865,446 @@
       </c>
       <c r="AQ38" s="10">
         <f>SUM(AQ13:AQ37)</f>
+        <v>14</v>
+      </c>
+      <c r="AR38" s="10"/>
+    </row>
+    <row r="40" spans="1:44">
+      <c r="B40" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="F40" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="12"/>
+      <c r="M40" s="12"/>
+      <c r="N40" s="12"/>
+      <c r="O40" s="12"/>
+      <c r="P40" s="12"/>
+      <c r="Q40" s="12"/>
+      <c r="R40" s="12"/>
+      <c r="S40" s="12"/>
+      <c r="T40" s="12"/>
+      <c r="U40" s="12"/>
+      <c r="V40" s="12"/>
+      <c r="W40" s="12"/>
+      <c r="X40" s="12"/>
+      <c r="Y40" s="12"/>
+      <c r="Z40" s="12"/>
+      <c r="AA40" s="12"/>
+      <c r="AB40" s="12"/>
+      <c r="AC40" s="12"/>
+      <c r="AD40" s="12"/>
+      <c r="AE40" s="12"/>
+      <c r="AF40" s="12"/>
+      <c r="AG40" s="12"/>
+      <c r="AH40" s="12"/>
+      <c r="AI40" s="12"/>
+      <c r="AJ40" s="12"/>
+      <c r="AK40" s="12"/>
+      <c r="AL40" s="12"/>
+      <c r="AM40" s="12"/>
+      <c r="AN40" s="12"/>
+      <c r="AO40" s="12"/>
+      <c r="AP40" s="12"/>
+      <c r="AQ40" s="12"/>
+      <c r="AR40" s="12"/>
+    </row>
+    <row r="41" spans="1:44">
+      <c r="B41" s="24">
+        <v>1</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" s="12">
+        <v>0</v>
+      </c>
+      <c r="F41" s="12">
+        <v>1</v>
+      </c>
+      <c r="G41" s="12" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve"/>
+          </r>
+          <r>
+            <rPr>
+              <rFont val="Calibri"/>
+              <b val="true"/>
+              <i val="false"/>
+              <strike val="false"/>
+              <color rgb="FF000000"/>
+              <sz val="11"/>
+              <u val="none"/>
+            </rPr>
+            <t xml:space="preserve">Viviendas: </t>
+          </r>
+          <r>
+            <t xml:space="preserve">si la vivienda no se pudo inspeccionar consignar C(vivienda cerrada), R(vivienda renuente) o D(vivienda deshabitada).</t>
+          </r>
+        </is>
+      </c>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
+      <c r="O41" s="12"/>
+      <c r="P41" s="12"/>
+      <c r="Q41" s="12"/>
+      <c r="R41" s="12"/>
+      <c r="S41" s="12"/>
+      <c r="T41" s="12"/>
+      <c r="U41" s="12"/>
+      <c r="V41" s="12"/>
+      <c r="W41" s="12"/>
+      <c r="X41" s="12"/>
+      <c r="Y41" s="12"/>
+      <c r="Z41" s="12"/>
+      <c r="AA41" s="12"/>
+      <c r="AB41" s="12"/>
+      <c r="AC41" s="12"/>
+      <c r="AD41" s="12"/>
+      <c r="AE41" s="12"/>
+      <c r="AF41" s="12"/>
+      <c r="AG41" s="12"/>
+      <c r="AH41" s="12"/>
+      <c r="AI41" s="12"/>
+      <c r="AJ41" s="12"/>
+      <c r="AK41" s="12"/>
+      <c r="AL41" s="12"/>
+      <c r="AM41" s="12"/>
+      <c r="AN41" s="12"/>
+      <c r="AO41" s="12"/>
+      <c r="AP41" s="12"/>
+      <c r="AQ41" s="12"/>
+      <c r="AR41" s="12"/>
+    </row>
+    <row r="42" spans="1:44">
+      <c r="B42" s="24">
+        <v>2</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42" s="12">
+        <v>0</v>
+      </c>
+      <c r="F42" s="12">
+        <v>2</v>
+      </c>
+      <c r="G42" s="12" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve"/>
+          </r>
+          <r>
+            <rPr>
+              <rFont val="Calibri"/>
+              <b val="true"/>
+              <i val="false"/>
+              <strike val="false"/>
+              <color rgb="FF000000"/>
+              <sz val="11"/>
+              <u val="none"/>
+            </rPr>
+            <t xml:space="preserve">Depositos: </t>
+          </r>
+          <r>
+            <t xml:space="preserve">en la columna: </t>
+          </r>
+          <r>
+            <rPr>
+              <rFont val="Calibri"/>
+              <b val="true"/>
+              <i val="false"/>
+              <strike val="false"/>
+              <color rgb="FF000000"/>
+              <sz val="11"/>
+              <u val="none"/>
+            </rPr>
+            <t xml:space="preserve">I</t>
+          </r>
+          <r>
+            <t xml:space="preserve">(inspeccionado), </t>
+          </r>
+          <r>
+            <rPr>
+              <rFont val="Calibri"/>
+              <b val="true"/>
+              <i val="false"/>
+              <strike val="false"/>
+              <color rgb="FF000000"/>
+              <sz val="11"/>
+              <u val="none"/>
+            </rPr>
+            <t xml:space="preserve">P</t>
+          </r>
+          <r>
+            <t xml:space="preserve">(positivo), </t>
+          </r>
+          <r>
+            <rPr>
+              <rFont val="Calibri"/>
+              <b val="true"/>
+              <i val="false"/>
+              <strike val="false"/>
+              <color rgb="FF000000"/>
+              <sz val="11"/>
+              <u val="none"/>
+            </rPr>
+            <t xml:space="preserve">TQ</t>
+          </r>
+          <r>
+            <t xml:space="preserve">(tratamiento fisico), </t>
+          </r>
+          <r>
+            <rPr>
+              <rFont val="Calibri"/>
+              <b val="true"/>
+              <i val="false"/>
+              <strike val="false"/>
+              <color rgb="FF000000"/>
+              <sz val="11"/>
+              <u val="none"/>
+            </rPr>
+            <t xml:space="preserve">D</t>
+          </r>
+          <r>
+            <t xml:space="preserve">(destruido), </t>
+          </r>
+          <r>
+            <t xml:space="preserve">colocar el número de recipientes segun corresponda.</t>
+          </r>
+        </is>
+      </c>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
+      <c r="K42" s="12"/>
+      <c r="L42" s="12"/>
+      <c r="M42" s="12"/>
+      <c r="N42" s="12"/>
+      <c r="O42" s="12"/>
+      <c r="P42" s="12"/>
+      <c r="Q42" s="12"/>
+      <c r="R42" s="12"/>
+      <c r="S42" s="12"/>
+      <c r="T42" s="12"/>
+      <c r="U42" s="12"/>
+      <c r="V42" s="12"/>
+      <c r="W42" s="12"/>
+      <c r="X42" s="12"/>
+      <c r="Y42" s="12"/>
+      <c r="Z42" s="12"/>
+      <c r="AA42" s="12"/>
+      <c r="AB42" s="12"/>
+      <c r="AC42" s="12"/>
+      <c r="AD42" s="12"/>
+      <c r="AE42" s="12"/>
+      <c r="AF42" s="12"/>
+      <c r="AG42" s="12"/>
+      <c r="AH42" s="12"/>
+      <c r="AI42" s="12"/>
+      <c r="AJ42" s="12"/>
+      <c r="AK42" s="12"/>
+      <c r="AL42" s="12"/>
+      <c r="AM42" s="12"/>
+      <c r="AN42" s="12"/>
+      <c r="AO42" s="12"/>
+      <c r="AP42" s="12"/>
+      <c r="AQ42" s="12"/>
+      <c r="AR42" s="12"/>
+    </row>
+    <row r="43" spans="1:44">
+      <c r="B43" s="24">
+        <v>3</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D43" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:44">
+      <c r="B44" s="24">
+        <v>4</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" s="12">
+        <v>0</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="22"/>
+      <c r="L44" s="22"/>
+      <c r="M44" s="22"/>
+      <c r="N44" s="22"/>
+      <c r="O44" s="17"/>
+      <c r="P44" s="17"/>
+      <c r="Q44" s="17"/>
+      <c r="R44" s="17"/>
+      <c r="S44" s="17"/>
+      <c r="T44" s="17"/>
+      <c r="U44" s="17"/>
+      <c r="V44" s="17"/>
+      <c r="W44" s="17"/>
+      <c r="X44" s="17"/>
+      <c r="Y44" s="17"/>
+      <c r="Z44" s="17"/>
+      <c r="AA44" s="17"/>
+      <c r="AB44" s="17"/>
+      <c r="AC44" s="17"/>
+      <c r="AD44" s="17"/>
+      <c r="AE44" s="17"/>
+      <c r="AF44" s="17"/>
+      <c r="AG44" s="17"/>
+      <c r="AH44" s="17"/>
+      <c r="AI44" s="17"/>
+      <c r="AJ44" s="17"/>
+      <c r="AK44" s="17"/>
+      <c r="AL44" s="17"/>
+      <c r="AM44" s="17"/>
+      <c r="AN44" s="17"/>
+      <c r="AO44" s="17"/>
+      <c r="AP44" s="17"/>
+      <c r="AQ44" s="17"/>
+      <c r="AR44" s="19"/>
+    </row>
+    <row r="45" spans="1:44">
+      <c r="B45" s="24">
         <v>5</v>
       </c>
-      <c r="AR38" s="10"/>
+      <c r="C45" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" s="12">
+        <v>0</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="18"/>
+      <c r="N45" s="18"/>
+      <c r="O45" s="13"/>
+      <c r="P45" s="13"/>
+      <c r="Q45" s="13"/>
+      <c r="R45" s="13"/>
+      <c r="S45" s="18"/>
+      <c r="T45" s="18"/>
+      <c r="U45" s="18"/>
+      <c r="V45" s="18"/>
+      <c r="W45" s="18"/>
+      <c r="X45" s="18"/>
+      <c r="Y45" s="18"/>
+      <c r="Z45" s="13"/>
+      <c r="AA45" s="13"/>
+      <c r="AB45" s="13"/>
+      <c r="AC45" s="13"/>
+      <c r="AD45" s="13"/>
+      <c r="AE45" s="13"/>
+      <c r="AF45" s="13"/>
+      <c r="AG45" s="13"/>
+      <c r="AH45" s="18"/>
+      <c r="AI45" s="18"/>
+      <c r="AJ45" s="18"/>
+      <c r="AK45" s="18"/>
+      <c r="AL45" s="18"/>
+      <c r="AM45" s="18"/>
+      <c r="AN45" s="18"/>
+      <c r="AO45" s="18"/>
+      <c r="AP45" s="13"/>
+      <c r="AQ45" s="13"/>
+      <c r="AR45" s="20"/>
+    </row>
+    <row r="46" spans="1:44">
+      <c r="B46" s="24">
+        <v>6</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" s="12">
+        <v>1</v>
+      </c>
+      <c r="F46" s="16"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="18"/>
+      <c r="M46" s="18"/>
+      <c r="N46" s="18"/>
+      <c r="O46" s="18"/>
+      <c r="P46" s="18"/>
+      <c r="Q46" s="18"/>
+      <c r="R46" s="18"/>
+      <c r="S46" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="T46" s="18"/>
+      <c r="U46" s="18"/>
+      <c r="V46" s="18"/>
+      <c r="W46" s="18"/>
+      <c r="X46" s="18"/>
+      <c r="Y46" s="18"/>
+      <c r="Z46" s="18"/>
+      <c r="AA46" s="18"/>
+      <c r="AB46" s="18"/>
+      <c r="AC46" s="18"/>
+      <c r="AD46" s="18"/>
+      <c r="AE46" s="18"/>
+      <c r="AF46" s="18"/>
+      <c r="AG46" s="18"/>
+      <c r="AH46" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI46" s="18"/>
+      <c r="AJ46" s="18"/>
+      <c r="AK46" s="18"/>
+      <c r="AL46" s="18"/>
+      <c r="AM46" s="18"/>
+      <c r="AN46" s="18"/>
+      <c r="AO46" s="18"/>
+      <c r="AP46" s="18"/>
+      <c r="AQ46" s="18"/>
+      <c r="AR46" s="21"/>
+    </row>
+    <row r="47" spans="1:44">
+      <c r="B47" s="24">
+        <v>7</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D47" s="12">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells>
@@ -2604,6 +3359,20 @@
     <mergeCell ref="AG10:AK11"/>
     <mergeCell ref="AL10:AP11"/>
     <mergeCell ref="A38:D38"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="F40:AR40"/>
+    <mergeCell ref="G41:AR41"/>
+    <mergeCell ref="G42:AR42"/>
+    <mergeCell ref="F43:AR43"/>
+    <mergeCell ref="F47:AR47"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="J44:N44"/>
+    <mergeCell ref="J45:N45"/>
+    <mergeCell ref="S45:Y45"/>
+    <mergeCell ref="S46:Y46"/>
+    <mergeCell ref="AH45:AO45"/>
+    <mergeCell ref="AH46:AO46"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true" horizontalCentered="true"/>
   <pageMargins left="0.472441" right="0.393701" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>